<commit_message>
corrected a path saving in a barcodes folder
</commit_message>
<xml_diff>
--- a/Python/Barcode Excell/barcodes.xlsx
+++ b/Python/Barcode Excell/barcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\cloud_garage_llp\Python\Barcode Excell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C568ED-72F2-4A2E-AAB4-7F507E606CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1AC880-3883-4AA3-BC90-A4A46BBC708E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DD6CC1F3-31FA-41F1-A5BD-38F8537D8425}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,39 +434,25 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>234567890123</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>345678901234</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>456789012345</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>567890123456</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>678901234567</v>
-      </c>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>789012345678</v>
-      </c>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>890123456789</v>
-      </c>
+      <c r="A11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>